<commit_message>
fixed all duplicate names, cleaned shooting, shot_creation and possession datasets
</commit_message>
<xml_diff>
--- a/data/league_data/england/20/england_defending.xlsx
+++ b/data/league_data/england/20/england_defending.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sanjitvarma/Desktop/trial_git/Predicting-Football-Player-Transfer-Values/data/league_data/england/20/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FA5516-4F91-A348-B4F0-E4283782BFDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14CD4BC6-307D-C649-90D4-2CF041D95202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1819,9 +1819,6 @@
     <t>Josh Martin</t>
   </si>
   <si>
-    <t>João Pedro</t>
-  </si>
-  <si>
     <t>Patrick Roberts</t>
   </si>
   <si>
@@ -1847,6 +1844,9 @@
   </si>
   <si>
     <t>Jota Peleteiro</t>
+  </si>
+  <si>
+    <t>João Pedro Junqueira</t>
   </si>
 </sst>
 </file>
@@ -2713,8 +2713,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A400" workbookViewId="0">
-      <selection activeCell="B415" sqref="B415"/>
+    <sheetView tabSelected="1" topLeftCell="A478" workbookViewId="0">
+      <selection activeCell="B493" sqref="B493"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -42057,7 +42057,7 @@
         <v>414</v>
       </c>
       <c r="B415" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="C415" s="3" t="s">
         <v>43</v>
@@ -49421,7 +49421,7 @@
         <v>492</v>
       </c>
       <c r="B493" s="3" t="s">
-        <v>599</v>
+        <v>608</v>
       </c>
       <c r="C493" s="3" t="s">
         <v>109</v>
@@ -49514,7 +49514,7 @@
         <v>493</v>
       </c>
       <c r="B494" s="3" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="C494" s="3" t="s">
         <v>28</v>
@@ -49607,7 +49607,7 @@
         <v>494</v>
       </c>
       <c r="B495" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="C495" s="3" t="s">
         <v>28</v>
@@ -49700,10 +49700,10 @@
         <v>495</v>
       </c>
       <c r="B496" s="3" t="s">
+        <v>601</v>
+      </c>
+      <c r="C496" s="3" t="s">
         <v>602</v>
-      </c>
-      <c r="C496" s="3" t="s">
-        <v>603</v>
       </c>
       <c r="D496" s="3" t="s">
         <v>53</v>
@@ -49793,7 +49793,7 @@
         <v>496</v>
       </c>
       <c r="B497" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
       <c r="C497" s="3" t="s">
         <v>28</v>
@@ -49886,7 +49886,7 @@
         <v>497</v>
       </c>
       <c r="B498" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
       <c r="C498" s="3" t="s">
         <v>43</v>
@@ -49981,7 +49981,7 @@
         <v>498</v>
       </c>
       <c r="B499" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
       <c r="C499" s="3" t="s">
         <v>28</v>
@@ -50074,7 +50074,7 @@
         <v>499</v>
       </c>
       <c r="B500" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
       <c r="C500" s="3" t="s">
         <v>170</v>

</xml_diff>